<commit_message>
Cleaning code and Adding Supplement
</commit_message>
<xml_diff>
--- a/supplementary_data/tables/Tasks_And_Datasets.xlsx
+++ b/supplementary_data/tables/Tasks_And_Datasets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/egg/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/egg/Projects/Stainalyzer/supplementary_data/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBADA32D-A7B7-CA48-B747-801B6C36729B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDACBA6C-FAF3-5748-8B0A-695CC0E3E268}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="820" yWindow="760" windowWidth="33740" windowHeight="21580" activeTab="1" xr2:uid="{31960518-8E6F-E64C-A266-0588CFE0860D}"/>
+    <workbookView xWindow="820" yWindow="500" windowWidth="33740" windowHeight="21100" xr2:uid="{31960518-8E6F-E64C-A266-0588CFE0860D}"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="245">
   <si>
     <t>Task</t>
   </si>
@@ -770,6 +770,9 @@
   </si>
   <si>
     <t>Total Images</t>
+  </si>
+  <si>
+    <t>Cell Types**</t>
   </si>
 </sst>
 </file>
@@ -1163,10 +1166,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{688C8998-1A91-0241-91CF-B1EF006B8561}">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1495,37 +1498,37 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>71</v>
+        <v>244</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E19" s="6" t="s">
-        <v>72</v>
+      <c r="E19" s="4" t="s">
+        <v>69</v>
       </c>
       <c r="F19" s="4"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E20" s="4" t="s">
-        <v>81</v>
+      <c r="E20" s="6" t="s">
+        <v>72</v>
       </c>
       <c r="F20" s="4"/>
     </row>
@@ -1537,7 +1540,7 @@
         <v>236</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>59</v>
@@ -1545,6 +1548,7 @@
       <c r="E21" s="4" t="s">
         <v>81</v>
       </c>
+      <c r="F21" s="4"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
@@ -1554,7 +1558,7 @@
         <v>236</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>59</v>
@@ -1571,7 +1575,7 @@
         <v>236</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>59</v>
@@ -1588,7 +1592,7 @@
         <v>236</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>59</v>
@@ -1605,7 +1609,7 @@
         <v>236</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>59</v>
@@ -1622,7 +1626,7 @@
         <v>236</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>59</v>
@@ -1639,7 +1643,7 @@
         <v>236</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>59</v>
@@ -1650,19 +1654,19 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>82</v>
+        <v>59</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -1673,12 +1677,29 @@
         <v>238</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>7</v>
       </c>
       <c r="E29" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" s="6" t="s">
         <v>82</v>
       </c>
     </row>
@@ -1691,7 +1712,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B75BE463-F411-C64B-B621-910E7BED33D9}">
   <dimension ref="A1:O12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
@@ -1699,8 +1720,8 @@
   <cols>
     <col min="1" max="1" width="26.1640625" style="6" customWidth="1"/>
     <col min="2" max="2" width="22.1640625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="12.83203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="28.1640625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="23.33203125" style="6" customWidth="1"/>
     <col min="5" max="5" width="12.5" style="6" customWidth="1"/>
     <col min="6" max="6" width="12" style="6" customWidth="1"/>
     <col min="7" max="7" width="17.6640625" style="6" customWidth="1"/>

</xml_diff>